<commit_message>
lab 13 format update
</commit_message>
<xml_diff>
--- a/labs/Lab_13_python_oop/solution/my_payments_analytics_2023_12_26.xlsx
+++ b/labs/Lab_13_python_oop/solution/my_payments_analytics_2023_12_26.xlsx
@@ -296,7 +296,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,16 +308,20 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -382,13 +386,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,172 +747,172 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -933,82 +940,82 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>